<commit_message>
removed old user stories
</commit_message>
<xml_diff>
--- a/6K185_DocShare_DayCare/Copy_NEWUpdated of Daycare_UserStories.xlsx
+++ b/6K185_DocShare_DayCare/Copy_NEWUpdated of Daycare_UserStories.xlsx
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="146">
   <si>
     <t>Story ID</t>
   </si>
@@ -783,6 +783,9 @@
   </si>
   <si>
     <t>S107</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1877,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,6 +1892,7 @@
     <col min="4" max="4" width="38.140625" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1979,6 +1983,9 @@
       <c r="H5" s="7" t="s">
         <v>107</v>
       </c>
+      <c r="K5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2041,6 +2048,9 @@
       <c r="H8" s="7" t="s">
         <v>110</v>
       </c>
+      <c r="K8" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2089,7 +2099,9 @@
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+      <c r="K13" s="17" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2192,7 +2204,9 @@
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="K19" s="17" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2318,7 +2332,9 @@
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
+      <c r="K26" s="17" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
@@ -2381,7 +2397,9 @@
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
+      <c r="K29" s="17" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
@@ -2402,7 +2420,9 @@
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
+      <c r="K30" s="17" t="s">
+        <v>145</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added names for user stories iteration 1
</commit_message>
<xml_diff>
--- a/6K185_DocShare_DayCare/Copy_NEWUpdated of Daycare_UserStories.xlsx
+++ b/6K185_DocShare_DayCare/Copy_NEWUpdated of Daycare_UserStories.xlsx
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="151">
   <si>
     <t>Story ID</t>
   </si>
@@ -786,6 +786,21 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Wyatt</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Waleed</t>
+  </si>
+  <si>
+    <t>Wyatt/David</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A40"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,6 +1973,9 @@
       <c r="H4" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="J4" s="17" t="s">
+        <v>147</v>
+      </c>
       <c r="K4" t="s">
         <v>103</v>
       </c>
@@ -1983,8 +2001,8 @@
       <c r="H5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="K5" t="s">
-        <v>145</v>
+      <c r="J5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2008,6 +2026,9 @@
       <c r="H6" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="J6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2026,6 +2047,9 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
+      <c r="J7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2068,6 +2092,12 @@
       <c r="G9" s="7" t="s">
         <v>115</v>
       </c>
+      <c r="J9" t="s">
+        <v>146</v>
+      </c>
+      <c r="K9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
@@ -2125,7 +2155,9 @@
         <v>111</v>
       </c>
       <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="J14" s="17" t="s">
+        <v>147</v>
+      </c>
       <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2230,7 +2262,9 @@
         <v>113</v>
       </c>
       <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="J20" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2255,7 +2289,9 @@
         <v>111</v>
       </c>
       <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="J21" s="17" t="s">
+        <v>147</v>
+      </c>
       <c r="K21" s="17" t="s">
         <v>103</v>
       </c>
@@ -2354,7 +2390,9 @@
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
+      <c r="J27" s="17" t="s">
+        <v>147</v>
+      </c>
       <c r="K27" s="17"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2376,7 +2414,9 @@
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
+      <c r="K28" s="17" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">

</xml_diff>